<commit_message>
made readme for assignments
</commit_message>
<xml_diff>
--- a/sessions/01-introduction/birds-eye-view.xlsx
+++ b/sessions/01-introduction/birds-eye-view.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/william_russell_mcgill_ca/Documents/Projects/epid-676/sessions/01-introduction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{686F27A7-44EE-A04E-A3E0-E03D03F3C441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{686F27A7-44EE-A04E-A3E0-E03D03F3C441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CB2656B-1701-5640-B27B-BD3B867F68BB}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-6700" windowWidth="51200" windowHeight="28300" xr2:uid="{0565A001-2CAE-9242-B663-FA03BFD2217E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{0565A001-2CAE-9242-B663-FA03BFD2217E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Programming assignments</t>
   </si>
@@ -43,16 +43,19 @@
     <t>Project proposal</t>
   </si>
   <si>
-    <t>Methods lectures</t>
-  </si>
-  <si>
-    <t>Application lectures</t>
-  </si>
-  <si>
     <t>Present open source pub</t>
   </si>
   <si>
     <t>Final project presentation</t>
+  </si>
+  <si>
+    <t>Methods + coding focus</t>
+  </si>
+  <si>
+    <t>Application focus</t>
+  </si>
+  <si>
+    <t>Final report due 4/21</t>
   </si>
 </sst>
 </file>
@@ -60,10 +63,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-1009]d/mmm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-1009]d/mmm/yy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -127,7 +138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -150,13 +161,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -166,7 +186,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -179,24 +199,27 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -220,22 +243,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>195792</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>100542</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>270934</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>94192</xdr:rowOff>
+      <xdr:rowOff>26000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB1A9C1E-75D7-1209-20DA-EC4A581D9DCC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EED22AD-BAB7-CF14-E9DE-A64037739439}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -251,8 +274,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="195792" y="2407709"/>
-          <a:ext cx="10071100" cy="1803400"/>
+          <a:off x="0" y="2730500"/>
+          <a:ext cx="7772400" cy="1448400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -561,24 +584,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D974BF3-BD84-E243-83F0-AC1EEE3CFBFB}">
-  <dimension ref="A1:AD29"/>
+  <dimension ref="A1:AC29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="30" width="3.5" customWidth="1"/>
-    <col min="31" max="31" width="7" customWidth="1"/>
+    <col min="2" max="28" width="3.5" customWidth="1"/>
+    <col min="29" max="29" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
     </row>
-    <row r="2" spans="1:30" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="13">
         <v>44930</v>
@@ -644,61 +667,50 @@
         <v>44981</v>
       </c>
       <c r="R2" s="13">
-        <f>Q2+5</f>
-        <v>44986</v>
+        <v>44993</v>
       </c>
       <c r="S2" s="13">
         <f>R2+2</f>
-        <v>44988</v>
+        <v>44995</v>
       </c>
       <c r="T2" s="5">
         <f>S2+5</f>
-        <v>44993</v>
+        <v>45000</v>
       </c>
       <c r="U2" s="5">
-        <f>T2+2</f>
-        <v>44995</v>
+        <f t="shared" ref="U2" si="0">T2+2</f>
+        <v>45002</v>
       </c>
       <c r="V2" s="13">
-        <f>U2+5</f>
-        <v>45000</v>
+        <f t="shared" ref="V2" si="1">U2+5</f>
+        <v>45007</v>
       </c>
       <c r="W2" s="13">
-        <f>V2+2</f>
-        <v>45002</v>
+        <f t="shared" ref="W2" si="2">V2+2</f>
+        <v>45009</v>
       </c>
       <c r="X2" s="5">
-        <f>W2+5</f>
-        <v>45007</v>
+        <f t="shared" ref="X2" si="3">W2+5</f>
+        <v>45014</v>
       </c>
       <c r="Y2" s="5">
-        <f>X2+2</f>
-        <v>45009</v>
+        <f t="shared" ref="Y2" si="4">X2+2</f>
+        <v>45016</v>
       </c>
       <c r="Z2" s="13">
-        <f>Y2+5</f>
-        <v>45014</v>
+        <f t="shared" ref="Z2" si="5">Y2+5</f>
+        <v>45021</v>
       </c>
       <c r="AA2" s="13">
-        <f>Z2+2</f>
-        <v>45016</v>
+        <v>45028</v>
       </c>
       <c r="AB2" s="5">
-        <f>AA2+5</f>
-        <v>45021</v>
-      </c>
-      <c r="AC2" s="5">
-        <f>AB2+2</f>
-        <v>45023</v>
-      </c>
-      <c r="AD2" s="13">
-        <f>AC2+5</f>
-        <v>45028</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+        <v>45029</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -727,10 +739,8 @@
       <c r="Z3" s="13"/>
       <c r="AA3" s="13"/>
       <c r="AB3" s="5"/>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="13"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
@@ -740,7 +750,9 @@
       <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
       <c r="E4" s="3">
         <v>2</v>
       </c>
@@ -756,8 +768,7 @@
       <c r="I4" s="3">
         <v>4</v>
       </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="4">
+      <c r="J4" s="4">
         <v>3</v>
       </c>
       <c r="L4" s="3">
@@ -783,12 +794,13 @@
       <c r="Z4" s="16"/>
       <c r="AA4" s="16"/>
       <c r="AB4" s="6"/>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="16"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AC4" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -808,7 +820,7 @@
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
       <c r="S5" s="11"/>
-      <c r="T5" s="6"/>
+      <c r="T5" s="11"/>
       <c r="U5" s="11"/>
       <c r="V5" s="11"/>
       <c r="W5" s="11"/>
@@ -817,10 +829,9 @@
       <c r="Z5" s="11"/>
       <c r="AA5" s="11"/>
       <c r="AB5" s="11"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="16"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AC5" s="17"/>
+    </row>
+    <row r="6" spans="1:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>1</v>
       </c>
@@ -833,8 +844,7 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="16"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="6"/>
+      <c r="L6" s="9"/>
       <c r="M6" s="6"/>
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
@@ -851,12 +861,11 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="16"/>
       <c r="AB6" s="6"/>
-      <c r="AC6" s="6"/>
-      <c r="AD6" s="16"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AC6" s="17"/>
+    </row>
+    <row r="7" spans="1:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -870,9 +879,9 @@
       <c r="K7" s="16"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
-      <c r="N7" s="16"/>
+      <c r="N7" s="9"/>
       <c r="O7" s="16"/>
-      <c r="P7" s="9"/>
+      <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="16"/>
       <c r="S7" s="16"/>
@@ -885,12 +894,11 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="16"/>
       <c r="AB7" s="6"/>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="16"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AC7" s="17"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -917,12 +925,11 @@
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
       <c r="Z8" s="16"/>
-      <c r="AA8" s="16"/>
+      <c r="AA8" s="8"/>
       <c r="AB8" s="6"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="16"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AC8" s="17"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -951,10 +958,8 @@
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
-      <c r="AC9" s="2"/>
-      <c r="AD9" s="2"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -983,10 +988,8 @@
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
-      <c r="AC10" s="2"/>
-      <c r="AD10" s="2"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1015,10 +1018,8 @@
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
-      <c r="AC11" s="2"/>
-      <c r="AD11" s="2"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1047,10 +1048,8 @@
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
-      <c r="AC12" s="2"/>
-      <c r="AD12" s="2"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1079,10 +1078,8 @@
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
-      <c r="AC13" s="2"/>
-      <c r="AD13" s="2"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1111,13 +1108,11 @@
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
-      <c r="AC14" s="2"/>
-      <c r="AD14" s="2"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -1160,10 +1155,13 @@
       <c r="A29" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="AC4:AC8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="D2 F2 H2 J2 L2 N2 P2 R2 T2 V2 X2 Z2 AB2" formula="1"/>
+    <ignoredError sqref="D2 F2 H2 J2 L2 N2 P2" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
tweaked syllabus, wrote most of session 1 slides
</commit_message>
<xml_diff>
--- a/sessions/01-introduction/birds-eye-view.xlsx
+++ b/sessions/01-introduction/birds-eye-view.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/william_russell_mcgill_ca/Documents/Projects/epid-676/sessions/01-introduction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{686F27A7-44EE-A04E-A3E0-E03D03F3C441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CB2656B-1701-5640-B27B-BD3B867F68BB}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="8_{686F27A7-44EE-A04E-A3E0-E03D03F3C441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2A34E02-DFC3-4249-A717-1100FB3CD5E7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{0565A001-2CAE-9242-B663-FA03BFD2217E}"/>
+    <workbookView xWindow="-51200" yWindow="-6700" windowWidth="51200" windowHeight="28300" xr2:uid="{0565A001-2CAE-9242-B663-FA03BFD2217E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,13 +49,13 @@
     <t>Final project presentation</t>
   </si>
   <si>
-    <t>Methods + coding focus</t>
+    <t>Final report due 4/21</t>
   </si>
   <si>
-    <t>Application focus</t>
+    <t>Methods phase</t>
   </si>
   <si>
-    <t>Final report due 4/21</t>
+    <t>Application phase</t>
   </si>
 </sst>
 </file>
@@ -65,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1009]d/mmm/yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -75,6 +75,14 @@
     </font>
     <font>
       <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -174,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -209,10 +217,7 @@
     <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -220,6 +225,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -244,21 +255,21 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>159377</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>26000</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>101958</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>13368</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EED22AD-BAB7-CF14-E9DE-A64037739439}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D189B79-7254-7FA3-B833-FCB9E6466AC2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -274,8 +285,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2730500"/>
-          <a:ext cx="7772400" cy="1448400"/>
+          <a:off x="0" y="2665956"/>
+          <a:ext cx="15589274" cy="2861886"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -586,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D974BF3-BD84-E243-83F0-AC1EEE3CFBFB}">
   <dimension ref="A1:AC29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="AC4" sqref="A2:AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,8 +720,8 @@
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>4</v>
+      <c r="A3" s="17" t="s">
+        <v>5</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -725,7 +736,7 @@
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
-      <c r="O3" s="13"/>
+      <c r="O3" s="10"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="13"/>
@@ -741,7 +752,7 @@
       <c r="AB3" s="5"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3">
@@ -771,51 +782,51 @@
       <c r="J4" s="4">
         <v>3</v>
       </c>
-      <c r="L4" s="3">
-        <v>5</v>
-      </c>
+      <c r="L4" s="6"/>
       <c r="M4" s="4">
         <v>4</v>
       </c>
-      <c r="N4" s="16"/>
-      <c r="O4" s="4">
+      <c r="N4" s="3">
         <v>5</v>
       </c>
-      <c r="P4" s="6"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="4">
+        <v>5</v>
+      </c>
       <c r="Q4" s="6"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
       <c r="X4" s="6"/>
       <c r="Y4" s="6"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="16"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15"/>
       <c r="AB4" s="6"/>
-      <c r="AC4" s="17" t="s">
+      <c r="AC4" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="11"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
@@ -829,105 +840,105 @@
       <c r="Z5" s="11"/>
       <c r="AA5" s="11"/>
       <c r="AB5" s="11"/>
-      <c r="AC5" s="17"/>
+      <c r="AC5" s="16"/>
     </row>
     <row r="6" spans="1:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="16"/>
+      <c r="J6" s="15"/>
       <c r="L6" s="9"/>
       <c r="M6" s="6"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
       <c r="T6" s="6"/>
       <c r="U6" s="6"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="16"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
-      <c r="Z6" s="16"/>
-      <c r="AA6" s="16"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
       <c r="AB6" s="6"/>
-      <c r="AC6" s="17"/>
+      <c r="AC6" s="16"/>
     </row>
     <row r="7" spans="1:29" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="9"/>
-      <c r="O7" s="16"/>
+      <c r="O7" s="15"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
       <c r="T7" s="8"/>
       <c r="U7" s="6"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
       <c r="X7" s="6"/>
       <c r="Y7" s="6"/>
-      <c r="Z7" s="16"/>
-      <c r="AA7" s="16"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="15"/>
       <c r="AB7" s="6"/>
-      <c r="AC7" s="17"/>
+      <c r="AC7" s="16"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
       <c r="T8" s="6"/>
       <c r="U8" s="6"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
-      <c r="Z8" s="16"/>
+      <c r="Z8" s="15"/>
       <c r="AA8" s="8"/>
       <c r="AB8" s="6"/>
-      <c r="AC8" s="17"/>
+      <c r="AC8" s="16"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>

</xml_diff>